<commit_message>
commands: sync process from pacakage.json to commands
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shun.cheung/Documents/learning/casualapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33EDFBB6-C1C3-9C48-AD5B-18977592F929}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63411972-C501-FE47-B7BA-4C4DD42661C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10460" yWindow="1000" windowWidth="17120" windowHeight="17000" xr2:uid="{D70ABF78-F301-B84D-BD2E-246F7AB1B5AF}"/>
+    <workbookView xWindow="3560" yWindow="460" windowWidth="24020" windowHeight="17540" xr2:uid="{D70ABF78-F301-B84D-BD2E-246F7AB1B5AF}"/>
   </bookViews>
   <sheets>
     <sheet name="application deploy commands" sheetId="13" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="50">
   <si>
     <t>Python</t>
   </si>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895829AB-853F-4A40-A4D0-66E43545364D}">
   <dimension ref="A2:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B26" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -755,8 +755,8 @@
         <v>28</v>
       </c>
       <c r="D12" t="str">
-        <f>"npm run build --prefix "&amp;$B$5 &amp; "/frontend"</f>
-        <v>npm run build --prefix /Users/shun.cheung/Documents/learning/casualapp/frontend</v>
+        <f>"cd "&amp;$B$5</f>
+        <v>cd /Users/shun.cheung/Documents/learning/casualapp</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -766,8 +766,8 @@
         <v>28</v>
       </c>
       <c r="D13" t="str">
-        <f>"npm run sync --prefix "&amp;$B$5 &amp; "/frontend"</f>
-        <v>npm run sync --prefix /Users/shun.cheung/Documents/learning/casualapp/frontend</v>
+        <f xml:space="preserve"> "cp -r backend " &amp; $B$4</f>
+        <v>cp -r backend 20190910-01</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -775,8 +775,8 @@
         <v>28</v>
       </c>
       <c r="D14" t="str">
-        <f>"cd "&amp;$B$5</f>
-        <v>cd /Users/shun.cheung/Documents/learning/casualapp</v>
+        <f>"npm run build --prefix "&amp;$B$5 &amp; "/frontend"</f>
+        <v>npm run build --prefix /Users/shun.cheung/Documents/learning/casualapp/frontend</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -784,8 +784,8 @@
         <v>28</v>
       </c>
       <c r="D15" t="str">
-        <f xml:space="preserve"> "cp -r backend " &amp; $B$4</f>
-        <v>cp -r backend 20190910-01</v>
+        <f>"touch "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/empty.txt &amp;&amp; rm -r "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/* &amp;&amp; rsync -av " &amp; $B$5 &amp;"/frontend/build/index.html "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/templates/. &amp;&amp; rsync -av --exclude='static' "  &amp; $B$5 &amp;"/frontend/build/* "&amp; $B$5 &amp;"/" &amp; $B$4&amp; "/base/static/. &amp;&amp; rsync -av " &amp; $B$5 &amp;"/frontend/build/static/* "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/."</f>
+        <v>touch /Users/shun.cheung/Documents/learning/casualapp/20190910-01/base/static/empty.txt &amp;&amp; rm -r /Users/shun.cheung/Documents/learning/casualapp/20190910-01/base/static/* &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/index.html /Users/shun.cheung/Documents/learning/casualapp/20190910-01/base/templates/. &amp;&amp; rsync -av --exclude='static' /Users/shun.cheung/Documents/learning/casualapp/frontend/build/* /Users/shun.cheung/Documents/learning/casualapp/20190910-01/base/static/. &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/static/* /Users/shun.cheung/Documents/learning/casualapp/20190910-01/base/static/.</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -811,44 +811,43 @@
         <v>28</v>
       </c>
       <c r="D18" t="str">
-        <f>"cd "&amp;$B$5&amp;"/"&amp;$B$4</f>
-        <v>cd /Users/shun.cheung/Documents/learning/casualapp/20190910-01</v>
+        <f>"python "&amp;$B$5&amp;"/"&amp;$B$4&amp;"/manage.py collectstatic"</f>
+        <v>python /Users/shun.cheung/Documents/learning/casualapp/20190910-01/manage.py collectstatic</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="C19" t="s">
         <v>28</v>
       </c>
-      <c r="D19" t="str">
-        <f>"python "&amp;$B$5&amp;"/"&amp;$B$4&amp;"/manage.py collectstatic"</f>
-        <v>python /Users/shun.cheung/Documents/learning/casualapp/20190910-01/manage.py collectstatic</v>
+      <c r="D19" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="C20" t="s">
         <v>28</v>
       </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="C21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" t="str">
+      <c r="D20" t="str">
         <f>"vi "&amp;$B$5&amp;"/"&amp;$B$4&amp;"/backend/settings.py"</f>
         <v>vi /Users/shun.cheung/Documents/learning/casualapp/20190910-01/backend/settings.py</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1"/>
+    <row r="22" spans="1:5" ht="15" customHeight="1">
+      <c r="C22" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" t="str">
+        <f>"cd "&amp;$B$5</f>
+        <v>cd /Users/shun.cheung/Documents/learning/casualapp</v>
+      </c>
+    </row>
     <row r="23" spans="1:5">
       <c r="C23" t="s">
         <v>28</v>
       </c>
       <c r="D23" t="str">
-        <f>"cd "&amp;$B$5</f>
-        <v>cd /Users/shun.cheung/Documents/learning/casualapp</v>
+        <f>"zip -r "&amp;$B$4&amp;".zip "&amp;$B$4</f>
+        <v>zip -r 20190910-01.zip 20190910-01</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -856,15 +855,6 @@
         <v>28</v>
       </c>
       <c r="D24" t="str">
-        <f>"zip -r "&amp;$B$4&amp;".zip "&amp;$B$4</f>
-        <v>zip -r 20190910-01.zip 20190910-01</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="C25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" t="str">
         <f>"rm -r "&amp;B4</f>
         <v>rm -r 20190910-01</v>
       </c>

</xml_diff>

<commit_message>
commands add celery commands
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shun.cheung/Documents/learning/casualapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B778F63E-0E39-0C44-A608-3C236E18128B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524222DC-89A8-F442-80D3-60A56E878CCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3560" yWindow="460" windowWidth="24020" windowHeight="17540" xr2:uid="{D70ABF78-F301-B84D-BD2E-246F7AB1B5AF}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
   <si>
     <t>Python</t>
   </si>
@@ -177,16 +177,28 @@
     <t>python /usr/local/casualapp/active/manage.py update_lookups</t>
   </si>
   <si>
-    <t>20190919-01</t>
-  </si>
-  <si>
     <t>beat tasks</t>
   </si>
   <si>
     <t>python /usr/local/casualapp/active/manage.py update_beat_tasks</t>
   </si>
   <si>
-    <t>uwsgi --ini uwsgi.ini</t>
+    <t>20190919-02</t>
+  </si>
+  <si>
+    <t>uwsgi --ini uwsgi.ini &amp;</t>
+  </si>
+  <si>
+    <t>celery -A backend beat -l info --scheduler  django_celery_beat.schedulers:DatabaseScheduler&amp;</t>
+  </si>
+  <si>
+    <t>celery -A backend worker -l info &amp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin </t>
+  </si>
+  <si>
+    <t>cd /usr/local/casualapp/active</t>
   </si>
 </sst>
 </file>
@@ -331,14 +343,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{895829AB-853F-4A40-A4D0-66E43545364D}">
   <dimension ref="A2:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -670,41 +682,41 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:6" ht="19">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="14"/>
+      <c r="C3" s="16"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="19">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="14"/>
+      <c r="B4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="16"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:6" ht="19">
       <c r="A5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="14"/>
+      <c r="C5" s="16"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="5"/>
@@ -784,7 +796,7 @@
       </c>
       <c r="D13" t="str">
         <f xml:space="preserve"> "cp -r backend " &amp; $B$4</f>
-        <v>cp -r backend 20190919-01</v>
+        <v>cp -r backend 20190919-02</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -802,7 +814,7 @@
       </c>
       <c r="D15" t="str">
         <f>"touch "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/empty.txt &amp;&amp; rm -r "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/* &amp;&amp; rsync -av " &amp; $B$5 &amp;"/frontend/build/index.html "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/templates/. &amp;&amp; rsync -av --exclude='static' "  &amp; $B$5 &amp;"/frontend/build/* "&amp; $B$5 &amp;"/" &amp; $B$4&amp; "/base/static/. &amp;&amp; rsync -av " &amp; $B$5 &amp;"/frontend/build/static/* "&amp;$B$5&amp;"/" &amp; $B$4&amp; "/base/static/."</f>
-        <v>touch /Users/shun.cheung/Documents/learning/casualapp/20190919-01/base/static/empty.txt &amp;&amp; rm -r /Users/shun.cheung/Documents/learning/casualapp/20190919-01/base/static/* &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/index.html /Users/shun.cheung/Documents/learning/casualapp/20190919-01/base/templates/. &amp;&amp; rsync -av --exclude='static' /Users/shun.cheung/Documents/learning/casualapp/frontend/build/* /Users/shun.cheung/Documents/learning/casualapp/20190919-01/base/static/. &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/static/* /Users/shun.cheung/Documents/learning/casualapp/20190919-01/base/static/.</v>
+        <v>touch /Users/shun.cheung/Documents/learning/casualapp/20190919-02/base/static/empty.txt &amp;&amp; rm -r /Users/shun.cheung/Documents/learning/casualapp/20190919-02/base/static/* &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/index.html /Users/shun.cheung/Documents/learning/casualapp/20190919-02/base/templates/. &amp;&amp; rsync -av --exclude='static' /Users/shun.cheung/Documents/learning/casualapp/frontend/build/* /Users/shun.cheung/Documents/learning/casualapp/20190919-02/base/static/. &amp;&amp; rsync -av /Users/shun.cheung/Documents/learning/casualapp/frontend/build/static/* /Users/shun.cheung/Documents/learning/casualapp/20190919-02/base/static/.</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -820,7 +832,7 @@
       </c>
       <c r="D17" t="str">
         <f>"pip freeze &gt; "&amp;$B$5 &amp;"/"&amp;$B$4&amp;"/requirement.txt"</f>
-        <v>pip freeze &gt; /Users/shun.cheung/Documents/learning/casualapp/20190919-01/requirement.txt</v>
+        <v>pip freeze &gt; /Users/shun.cheung/Documents/learning/casualapp/20190919-02/requirement.txt</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -829,7 +841,7 @@
       </c>
       <c r="D18" t="str">
         <f>"python "&amp;$B$5&amp;"/"&amp;$B$4&amp;"/manage.py collectstatic"</f>
-        <v>python /Users/shun.cheung/Documents/learning/casualapp/20190919-01/manage.py collectstatic</v>
+        <v>python /Users/shun.cheung/Documents/learning/casualapp/20190919-02/manage.py collectstatic</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -846,7 +858,7 @@
       </c>
       <c r="D20" t="str">
         <f>"vi "&amp;$B$5&amp;"/"&amp;$B$4&amp;"/backend/settings.py"</f>
-        <v>vi /Users/shun.cheung/Documents/learning/casualapp/20190919-01/backend/settings.py</v>
+        <v>vi /Users/shun.cheung/Documents/learning/casualapp/20190919-02/backend/settings.py</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1">
@@ -864,7 +876,7 @@
       </c>
       <c r="D23" t="str">
         <f>"zip -r "&amp;$B$4&amp;".zip "&amp;$B$4</f>
-        <v>zip -r 20190919-01.zip 20190919-01</v>
+        <v>zip -r 20190919-02.zip 20190919-02</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -873,7 +885,7 @@
       </c>
       <c r="D24" t="str">
         <f>"rm -r "&amp;B4</f>
-        <v>rm -r 20190919-01</v>
+        <v>rm -r 20190919-02</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -908,7 +920,7 @@
       </c>
       <c r="D30" t="str">
         <f>"put "&amp;B4&amp;".zip"</f>
-        <v>put 20190919-01.zip</v>
+        <v>put 20190919-02.zip</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -925,7 +937,7 @@
       </c>
       <c r="D33" t="str">
         <f>"rm -r "&amp;B4 &amp; ".zip"</f>
-        <v>rm -r 20190919-01.zip</v>
+        <v>rm -r 20190919-02.zip</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -948,7 +960,7 @@
       </c>
       <c r="D36" t="str">
         <f>"mv " &amp; $B$4 &amp;".zip /usr/local/casualapp/"</f>
-        <v>mv 20190919-01.zip /usr/local/casualapp/</v>
+        <v>mv 20190919-02.zip /usr/local/casualapp/</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -965,7 +977,7 @@
       </c>
       <c r="D38" t="str">
         <f>"unzip /usr/local/casualapp/"&amp;$B$4&amp;".zip -d ."</f>
-        <v>unzip /usr/local/casualapp/20190919-01.zip -d .</v>
+        <v>unzip /usr/local/casualapp/20190919-02.zip -d .</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -977,7 +989,7 @@
       </c>
       <c r="D39" t="str">
         <f>"ln -sfn /usr/local/casualapp/"&amp;$B$4&amp;" /usr/local/casualapp/active"</f>
-        <v>ln -sfn /usr/local/casualapp/20190919-01 /usr/local/casualapp/active</v>
+        <v>ln -sfn /usr/local/casualapp/20190919-02 /usr/local/casualapp/active</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1076,13 +1088,13 @@
     </row>
     <row r="49" spans="1:5">
       <c r="B49" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D49" s="10" t="s">
         <v>50</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1099,47 +1111,63 @@
     <row r="52" spans="1:5">
       <c r="A52" s="2"/>
       <c r="C52" s="2" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E52" s="2"/>
     </row>
     <row r="53" spans="1:5">
       <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="E53" s="2"/>
     </row>
     <row r="54" spans="1:5">
+      <c r="C54" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D54" t="s">
+        <v>53</v>
+      </c>
       <c r="E54" s="2"/>
     </row>
-    <row r="56" spans="1:5">
-      <c r="C56" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D56" s="16" t="s">
+    <row r="55" spans="1:5">
+      <c r="C55" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="C57" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
-      <c r="C57" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D57" s="16" t="s">
+    <row r="58" spans="1:5">
+      <c r="C58" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
-      <c r="C58" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D58" s="15" t="s">
+    <row r="59" spans="1:5">
+      <c r="C59" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D59" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E53" xr:uid="{A8B3ADA8-34F4-324A-9A28-A5521834AEBA}"/>

</xml_diff>